<commit_message>
Update the changes for exercise 2
</commit_message>
<xml_diff>
--- a/starter-analysis-exercise/data/raw-data/exampledata.xlsx
+++ b/starter-analysis-exercise/data/raw-data/exampledata.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11210"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA1B0400-91DC-4479-905F-9A91D902E8D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7729956A-2172-F947-AB4E-06823344C29C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3555" yWindow="945" windowWidth="48840" windowHeight="21645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="620" yWindow="940" windowWidth="35380" windowHeight="21640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="27">
   <si>
     <t>Height</t>
   </si>
@@ -72,13 +72,43 @@
   </si>
   <si>
     <t>identified gender (male/female/other)</t>
+  </si>
+  <si>
+    <t>age</t>
+  </si>
+  <si>
+    <t>Educ</t>
+  </si>
+  <si>
+    <t>College</t>
+  </si>
+  <si>
+    <t>High school</t>
+  </si>
+  <si>
+    <t>Undergraduate</t>
+  </si>
+  <si>
+    <t>Graduate</t>
+  </si>
+  <si>
+    <t>age in complete years</t>
+  </si>
+  <si>
+    <t>educ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">level of education </t>
+  </si>
+  <si>
+    <t>Highschool,college, undergrate, Graduate</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -93,6 +123,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF374151"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -115,9 +151,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -398,174 +447,268 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="3" width="9.1640625" style="3"/>
+    <col min="5" max="5" width="12.5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="D1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="3">
         <v>180</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="3">
         <v>80</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="D2">
+        <v>50</v>
+      </c>
+      <c r="E2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="3">
         <v>175</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="3">
         <v>70</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="D3">
+        <v>45</v>
+      </c>
+      <c r="E3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="3">
         <v>60</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="D4">
+        <v>65</v>
+      </c>
+      <c r="E4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="3">
         <v>178</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="3">
         <v>76</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6">
+      <c r="D5">
+        <v>56</v>
+      </c>
+      <c r="E5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="3">
         <v>192</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="3">
         <v>90</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7">
+      <c r="D6">
+        <v>36</v>
+      </c>
+      <c r="E6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="3">
         <v>6</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="3">
         <v>55</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8">
+      <c r="D7">
+        <v>54</v>
+      </c>
+      <c r="E7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="3">
         <v>156</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="3">
         <v>90</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9">
+      <c r="D8">
+        <v>34</v>
+      </c>
+      <c r="E8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="3">
         <v>166</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="3">
         <v>110</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10">
+      <c r="D9">
+        <v>38</v>
+      </c>
+      <c r="E9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="3">
         <v>155</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="3">
         <v>54</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11">
+      <c r="D10">
+        <v>30</v>
+      </c>
+      <c r="E10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="3">
         <v>145</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="3">
         <v>7000</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12">
+      <c r="D11">
+        <v>42</v>
+      </c>
+      <c r="E11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="3">
         <v>165</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13">
+      <c r="D12">
+        <v>44</v>
+      </c>
+      <c r="E12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="3">
         <v>133</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="3">
         <v>45</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14">
+      <c r="D13">
+        <v>22</v>
+      </c>
+      <c r="E13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="3">
         <v>166</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="3">
         <v>55</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15">
+      <c r="D14">
+        <v>54</v>
+      </c>
+      <c r="E14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="3">
         <v>154</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="3">
         <v>50</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="3" t="s">
         <v>3</v>
+      </c>
+      <c r="D15">
+        <v>22</v>
+      </c>
+      <c r="E15" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -575,20 +718,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4A2C8F0-62B4-4D60-B490-D490A3E0B40F}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C9:C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.28515625" customWidth="1"/>
-    <col min="3" max="3" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="99.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -599,7 +742,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -610,7 +753,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -621,7 +764,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -631,9 +774,369 @@
       <c r="C4" t="s">
         <v>14</v>
       </c>
+    </row>
+    <row r="5" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="C7" s="5"/>
+    </row>
+    <row r="8" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="C8" s="5"/>
+    </row>
+    <row r="9" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="C9" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_activity xmlns="e3b1676e-f667-438e-893d-cb04b311f346" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010093A5F9A029148A4EBCB006CAE1D64BB0" ma:contentTypeVersion="19" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b77b9c52c0ff25a89b055ab00881b595">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns3="e3b1676e-f667-438e-893d-cb04b311f346" xmlns:ns4="eeaf2bdc-5f2b-4e0a-9255-c018dcc5488a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7599683d23761b1bb0c1ebb20061c5d4" ns1:_="" ns3:_="" ns4:_="">
+    <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
+    <xsd:import namespace="e3b1676e-f667-438e-893d-cb04b311f346"/>
+    <xsd:import namespace="eeaf2bdc-5f2b-4e0a-9255-c018dcc5488a"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns3:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceAutoKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceObjectDetectorVersions" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceAutoTags" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns3:_activity" minOccurs="0"/>
+                <xsd:element ref="ns4:SharedWithUsers" minOccurs="0"/>
+                <xsd:element ref="ns4:SharedWithDetails" minOccurs="0"/>
+                <xsd:element ref="ns4:SharingHintHash" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaLengthInSeconds" minOccurs="0"/>
+                <xsd:element ref="ns1:_ip_UnifiedCompliancePolicyProperties" minOccurs="0"/>
+                <xsd:element ref="ns1:_ip_UnifiedCompliancePolicyUIAction" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceSystemTags" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceSearchProperties" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="http://schemas.microsoft.com/sharepoint/v3" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="_ip_UnifiedCompliancePolicyProperties" ma:index="23" nillable="true" ma:displayName="Unified Compliance Policy Properties" ma:hidden="true" ma:internalName="_ip_UnifiedCompliancePolicyProperties">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="_ip_UnifiedCompliancePolicyUIAction" ma:index="24" nillable="true" ma:displayName="Unified Compliance Policy UI Action" ma:hidden="true" ma:internalName="_ip_UnifiedCompliancePolicyUIAction">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="e3b1676e-f667-438e-893d-cb04b311f346" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoKeyPoints" ma:index="10" nillable="true" ma:displayName="MediaServiceAutoKeyPoints" ma:hidden="true" ma:internalName="MediaServiceAutoKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceKeyPoints" ma:index="11" nillable="true" ma:displayName="KeyPoints" ma:internalName="MediaServiceKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="12" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoTags" ma:index="13" nillable="true" ma:displayName="Tags" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="14" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="15" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="16" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="_activity" ma:index="17" nillable="true" ma:displayName="_activity" ma:hidden="true" ma:internalName="_activity">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="21" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaLengthInSeconds" ma:index="22" nillable="true" ma:displayName="MediaLengthInSeconds" ma:hidden="true" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceSystemTags" ma:index="25" nillable="true" ma:displayName="MediaServiceSystemTags" ma:hidden="true" ma:internalName="MediaServiceSystemTags" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceSearchProperties" ma:index="26" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="eeaf2bdc-5f2b-4e0a-9255-c018dcc5488a" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="SharedWithUsers" ma:index="18" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:UserMulti">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="SharedWithDetails" ma:index="19" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="SharingHintHash" ma:index="20" nillable="true" ma:displayName="Sharing Hint Hash" ma:hidden="true" ma:internalName="SharingHintHash" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CEB28A1F-557E-4DB0-96B7-5ABC2156427E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="eeaf2bdc-5f2b-4e0a-9255-c018dcc5488a"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="e3b1676e-f667-438e-893d-cb04b311f346"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{51DCF06B-1466-4339-B6E5-B10BB8A80156}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="e3b1676e-f667-438e-893d-cb04b311f346"/>
+    <ds:schemaRef ds:uri="eeaf2bdc-5f2b-4e0a-9255-c018dcc5488a"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B55671CD-2998-4442-82A1-A91793A53477}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>